<commit_message>
Refactored, the final version max train size was modified
</commit_message>
<xml_diff>
--- a/data/output/Wind_data_predict.xlsx
+++ b/data/output/Wind_data_predict.xlsx
@@ -456,7 +456,7 @@
         <v>43839</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0237349160015583</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         <v>43839.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02375230565667152</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         <v>43839.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02396102622151375</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         <v>43839.125</v>
       </c>
       <c r="B5" t="n">
-        <v>0.02189065515995026</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         <v>43839.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>0.03774430602788925</v>
+        <v>0.04261558502912521</v>
       </c>
     </row>
     <row r="7">
@@ -496,7 +496,7 @@
         <v>43839.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04116721823811531</v>
+        <v>0.03100503422319889</v>
       </c>
     </row>
     <row r="8">
@@ -504,7 +504,7 @@
         <v>43839.25</v>
       </c>
       <c r="B8" t="n">
-        <v>0.08763329684734344</v>
+        <v>0.07880202680826187</v>
       </c>
     </row>
     <row r="9">
@@ -512,7 +512,7 @@
         <v>43839.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1402779221534729</v>
+        <v>0.1343789994716644</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +520,7 @@
         <v>43839.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1614013165235519</v>
+        <v>0.1469141393899918</v>
       </c>
     </row>
     <row r="11">
@@ -528,7 +528,7 @@
         <v>43839.375</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1275803595781326</v>
+        <v>0.1000665202736855</v>
       </c>
     </row>
     <row r="12">
@@ -536,7 +536,7 @@
         <v>43839.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>0.04398119822144508</v>
+        <v>0.03529689833521843</v>
       </c>
     </row>
     <row r="13">
@@ -544,7 +544,7 @@
         <v>43839.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>0.01888870261609554</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="14">
@@ -552,7 +552,7 @@
         <v>43839.5</v>
       </c>
       <c r="B14" t="n">
-        <v>0.04123217985033989</v>
+        <v>0.04917032644152641</v>
       </c>
     </row>
     <row r="15">
@@ -560,7 +560,7 @@
         <v>43839.54166666666</v>
       </c>
       <c r="B15" t="n">
-        <v>0.04711556434631348</v>
+        <v>0.05099577829241753</v>
       </c>
     </row>
     <row r="16">
@@ -568,7 +568,7 @@
         <v>43839.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>0.08249576389789581</v>
+        <v>0.04806243255734444</v>
       </c>
     </row>
     <row r="17">
@@ -576,7 +576,7 @@
         <v>43839.625</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2205421626567841</v>
+        <v>0.1717489510774612</v>
       </c>
     </row>
     <row r="18">
@@ -584,7 +584,7 @@
         <v>43839.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3858639001846313</v>
+        <v>0.3450882434844971</v>
       </c>
     </row>
     <row r="19">
@@ -592,7 +592,7 @@
         <v>43839.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4320091903209686</v>
+        <v>0.3895267844200134</v>
       </c>
     </row>
     <row r="20">
@@ -600,7 +600,7 @@
         <v>43839.75</v>
       </c>
       <c r="B20" t="n">
-        <v>0.4500717520713806</v>
+        <v>0.3939395546913147</v>
       </c>
     </row>
     <row r="21">
@@ -608,7 +608,7 @@
         <v>43839.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>0.420004814863205</v>
+        <v>0.3837548196315765</v>
       </c>
     </row>
     <row r="22">
@@ -616,7 +616,7 @@
         <v>43839.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>0.42157381772995</v>
+        <v>0.3795405924320221</v>
       </c>
     </row>
     <row r="23">
@@ -624,7 +624,7 @@
         <v>43839.875</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4488075077533722</v>
+        <v>0.3858906328678131</v>
       </c>
     </row>
     <row r="24">
@@ -632,7 +632,7 @@
         <v>43839.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3593409061431885</v>
+        <v>0.3736143708229065</v>
       </c>
     </row>
     <row r="25">
@@ -640,7 +640,7 @@
         <v>43839.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>0.4261586964130402</v>
+        <v>0.3833216726779938</v>
       </c>
     </row>
     <row r="26">
@@ -648,7 +648,7 @@
         <v>43840</v>
       </c>
       <c r="B26" t="n">
-        <v>0.4136970937252045</v>
+        <v>0.3875951766967773</v>
       </c>
     </row>
     <row r="27">
@@ -656,7 +656,7 @@
         <v>43840.04166666666</v>
       </c>
       <c r="B27" t="n">
-        <v>0.4253004789352417</v>
+        <v>0.3941161930561066</v>
       </c>
     </row>
     <row r="28">
@@ -664,7 +664,7 @@
         <v>43840.08333333334</v>
       </c>
       <c r="B28" t="n">
-        <v>0.4155730009078979</v>
+        <v>0.3946114480495453</v>
       </c>
     </row>
     <row r="29">
@@ -672,7 +672,7 @@
         <v>43840.125</v>
       </c>
       <c r="B29" t="n">
-        <v>0.4141563177108765</v>
+        <v>0.394012063741684</v>
       </c>
     </row>
     <row r="30">
@@ -680,7 +680,7 @@
         <v>43840.16666666666</v>
       </c>
       <c r="B30" t="n">
-        <v>0.4105978012084961</v>
+        <v>0.3729609847068787</v>
       </c>
     </row>
     <row r="31">
@@ -688,7 +688,7 @@
         <v>43840.20833333334</v>
       </c>
       <c r="B31" t="n">
-        <v>0.3206959068775177</v>
+        <v>0.3054832220077515</v>
       </c>
     </row>
     <row r="32">
@@ -696,7 +696,7 @@
         <v>43840.25</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2744612395763397</v>
+        <v>0.2029432356357574</v>
       </c>
     </row>
     <row r="33">
@@ -704,7 +704,7 @@
         <v>43840.29166666666</v>
       </c>
       <c r="B33" t="n">
-        <v>0.1197403073310852</v>
+        <v>0.08896761387586594</v>
       </c>
     </row>
     <row r="34">
@@ -712,7 +712,7 @@
         <v>43840.33333333334</v>
       </c>
       <c r="B34" t="n">
-        <v>0.06834867596626282</v>
+        <v>0.05902456119656563</v>
       </c>
     </row>
     <row r="35">
@@ -720,7 +720,7 @@
         <v>43840.375</v>
       </c>
       <c r="B35" t="n">
-        <v>0.08876258879899979</v>
+        <v>0.0827145054936409</v>
       </c>
     </row>
     <row r="36">
@@ -728,7 +728,7 @@
         <v>43840.41666666666</v>
       </c>
       <c r="B36" t="n">
-        <v>0.08828005939722061</v>
+        <v>0.07151544839143753</v>
       </c>
     </row>
     <row r="37">
@@ -736,7 +736,7 @@
         <v>43840.45833333334</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1207593902945518</v>
+        <v>0.1140044629573822</v>
       </c>
     </row>
     <row r="38">
@@ -744,7 +744,7 @@
         <v>43840.5</v>
       </c>
       <c r="B38" t="n">
-        <v>0.1206203997135162</v>
+        <v>0.1185560449957848</v>
       </c>
     </row>
     <row r="39">
@@ -752,7 +752,7 @@
         <v>43840.54166666666</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1543852835893631</v>
+        <v>0.1265325099229813</v>
       </c>
     </row>
     <row r="40">
@@ -760,7 +760,7 @@
         <v>43840.58333333334</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1145694404840469</v>
+        <v>0.1185560449957848</v>
       </c>
     </row>
     <row r="41">
@@ -768,7 +768,7 @@
         <v>43840.625</v>
       </c>
       <c r="B41" t="n">
-        <v>0.09857632219791412</v>
+        <v>0.07957780361175537</v>
       </c>
     </row>
     <row r="42">
@@ -776,7 +776,7 @@
         <v>43840.66666666666</v>
       </c>
       <c r="B42" t="n">
-        <v>0.04870476573705673</v>
+        <v>0.04900955781340599</v>
       </c>
     </row>
     <row r="43">
@@ -784,7 +784,7 @@
         <v>43840.70833333334</v>
       </c>
       <c r="B43" t="n">
-        <v>0.04363028332591057</v>
+        <v>0.04671235382556915</v>
       </c>
     </row>
     <row r="44">
@@ -792,7 +792,7 @@
         <v>43840.75</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0441250391304493</v>
+        <v>0.04671235382556915</v>
       </c>
     </row>
     <row r="45">
@@ -800,7 +800,7 @@
         <v>43840.79166666666</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0441027395427227</v>
+        <v>0.04671235382556915</v>
       </c>
     </row>
     <row r="46">
@@ -808,7 +808,7 @@
         <v>43840.83333333334</v>
       </c>
       <c r="B46" t="n">
-        <v>0.04166250303387642</v>
+        <v>0.04671235382556915</v>
       </c>
     </row>
     <row r="47">
@@ -816,7 +816,7 @@
         <v>43840.875</v>
       </c>
       <c r="B47" t="n">
-        <v>0.03994135558605194</v>
+        <v>0.0408606268465519</v>
       </c>
     </row>
     <row r="48">
@@ -824,7 +824,7 @@
         <v>43840.91666666666</v>
       </c>
       <c r="B48" t="n">
-        <v>0.03083853982388973</v>
+        <v>0.03269428387284279</v>
       </c>
     </row>
     <row r="49">
@@ -832,7 +832,7 @@
         <v>43840.95833333334</v>
       </c>
       <c r="B49" t="n">
-        <v>0.02825540862977505</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="50">
@@ -840,7 +840,7 @@
         <v>43841</v>
       </c>
       <c r="B50" t="n">
-        <v>0.03428114950656891</v>
+        <v>0.03549665212631226</v>
       </c>
     </row>
     <row r="51">
@@ -848,7 +848,7 @@
         <v>43841.04166666666</v>
       </c>
       <c r="B51" t="n">
-        <v>0.04098930954933167</v>
+        <v>0.04261558502912521</v>
       </c>
     </row>
     <row r="52">
@@ -856,7 +856,7 @@
         <v>43841.08333333334</v>
       </c>
       <c r="B52" t="n">
-        <v>0.03259256482124329</v>
+        <v>0.03549665212631226</v>
       </c>
     </row>
     <row r="53">
@@ -864,7 +864,7 @@
         <v>43841.125</v>
       </c>
       <c r="B53" t="n">
-        <v>0.02327604405581951</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="54">
@@ -872,7 +872,7 @@
         <v>43841.16666666666</v>
       </c>
       <c r="B54" t="n">
-        <v>0.02697617933154106</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="55">
@@ -880,7 +880,7 @@
         <v>43841.20833333334</v>
       </c>
       <c r="B55" t="n">
-        <v>0.02907135710120201</v>
+        <v>0.02856598980724812</v>
       </c>
     </row>
     <row r="56">
@@ -888,7 +888,7 @@
         <v>43841.25</v>
       </c>
       <c r="B56" t="n">
-        <v>0.02971568703651428</v>
+        <v>0.02856598980724812</v>
       </c>
     </row>
     <row r="57">
@@ -896,7 +896,7 @@
         <v>43841.29166666666</v>
       </c>
       <c r="B57" t="n">
-        <v>0.02760959975421429</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="58">
@@ -904,7 +904,7 @@
         <v>43841.33333333334</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0235917940735817</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="59">
@@ -912,7 +912,7 @@
         <v>43841.375</v>
       </c>
       <c r="B59" t="n">
-        <v>0.02543263137340546</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="60">
@@ -920,7 +920,7 @@
         <v>43841.41666666666</v>
       </c>
       <c r="B60" t="n">
-        <v>0.02381692640483379</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="61">
@@ -928,7 +928,7 @@
         <v>43841.45833333334</v>
       </c>
       <c r="B61" t="n">
-        <v>0.02478807233273983</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="62">
@@ -936,7 +936,7 @@
         <v>43841.5</v>
       </c>
       <c r="B62" t="n">
-        <v>0.02693326957523823</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="63">
@@ -944,7 +944,7 @@
         <v>43841.54166666666</v>
       </c>
       <c r="B63" t="n">
-        <v>0.02381692640483379</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="64">
@@ -952,7 +952,7 @@
         <v>43841.58333333334</v>
       </c>
       <c r="B64" t="n">
-        <v>0.02277394570410252</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="65">
@@ -960,7 +960,7 @@
         <v>43841.625</v>
       </c>
       <c r="B65" t="n">
-        <v>0.02174869738519192</v>
+        <v>0.02820187248289585</v>
       </c>
     </row>
     <row r="66">
@@ -968,7 +968,7 @@
         <v>43841.66666666666</v>
       </c>
       <c r="B66" t="n">
-        <v>0.01601923070847988</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="67">
@@ -976,7 +976,7 @@
         <v>43841.70833333334</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0191977433860302</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="68">
@@ -984,7 +984,7 @@
         <v>43841.75</v>
       </c>
       <c r="B68" t="n">
-        <v>0.04597610980272293</v>
+        <v>0.03539891168475151</v>
       </c>
     </row>
     <row r="69">
@@ -992,7 +992,7 @@
         <v>43841.79166666666</v>
       </c>
       <c r="B69" t="n">
-        <v>0.0816711038351059</v>
+        <v>0.08561854809522629</v>
       </c>
     </row>
     <row r="70">
@@ -1000,7 +1000,7 @@
         <v>43841.83333333334</v>
       </c>
       <c r="B70" t="n">
-        <v>0.1034000217914581</v>
+        <v>0.1005492806434631</v>
       </c>
     </row>
     <row r="71">
@@ -1008,7 +1008,7 @@
         <v>43841.875</v>
       </c>
       <c r="B71" t="n">
-        <v>0.08024351298809052</v>
+        <v>0.09617377817630768</v>
       </c>
     </row>
     <row r="72">
@@ -1016,7 +1016,7 @@
         <v>43841.91666666666</v>
       </c>
       <c r="B72" t="n">
-        <v>0.06241609156131744</v>
+        <v>0.0614122599363327</v>
       </c>
     </row>
     <row r="73">
@@ -1024,7 +1024,7 @@
         <v>43841.95833333334</v>
       </c>
       <c r="B73" t="n">
-        <v>0.05149208381772041</v>
+        <v>0.04922284558415413</v>
       </c>
     </row>
     <row r="74">
@@ -1032,7 +1032,7 @@
         <v>43842</v>
       </c>
       <c r="B74" t="n">
-        <v>0.04920481517910957</v>
+        <v>0.04117486998438835</v>
       </c>
     </row>
     <row r="75">
@@ -1040,7 +1040,7 @@
         <v>43842.04166666666</v>
       </c>
       <c r="B75" t="n">
-        <v>0.04734934866428375</v>
+        <v>0.04647859930992126</v>
       </c>
     </row>
     <row r="76">
@@ -1048,7 +1048,7 @@
         <v>43842.08333333334</v>
       </c>
       <c r="B76" t="n">
-        <v>0.04234904423356056</v>
+        <v>0.04647859930992126</v>
       </c>
     </row>
     <row r="77">
@@ -1056,7 +1056,7 @@
         <v>43842.125</v>
       </c>
       <c r="B77" t="n">
-        <v>0.05893014743924141</v>
+        <v>0.07439888268709183</v>
       </c>
     </row>
     <row r="78">
@@ -1064,7 +1064,7 @@
         <v>43842.16666666666</v>
       </c>
       <c r="B78" t="n">
-        <v>0.05947105213999748</v>
+        <v>0.0592782236635685</v>
       </c>
     </row>
     <row r="79">
@@ -1072,7 +1072,7 @@
         <v>43842.20833333334</v>
       </c>
       <c r="B79" t="n">
-        <v>0.05063972249627113</v>
+        <v>0.04963897541165352</v>
       </c>
     </row>
     <row r="80">
@@ -1080,7 +1080,7 @@
         <v>43842.25</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0460347905755043</v>
+        <v>0.03819409385323524</v>
       </c>
     </row>
     <row r="81">
@@ -1088,7 +1088,7 @@
         <v>43842.29166666666</v>
       </c>
       <c r="B81" t="n">
-        <v>0.04621095210313797</v>
+        <v>0.03543885797262192</v>
       </c>
     </row>
     <row r="82">
@@ -1096,7 +1096,7 @@
         <v>43842.33333333334</v>
       </c>
       <c r="B82" t="n">
-        <v>0.04791337251663208</v>
+        <v>0.0371975488960743</v>
       </c>
     </row>
     <row r="83">
@@ -1104,7 +1104,7 @@
         <v>43842.375</v>
       </c>
       <c r="B83" t="n">
-        <v>0.03972334042191505</v>
+        <v>0.03068605065345764</v>
       </c>
     </row>
     <row r="84">
@@ -1112,7 +1112,7 @@
         <v>43842.41666666666</v>
       </c>
       <c r="B84" t="n">
-        <v>0.04202940687537193</v>
+        <v>0.03068605065345764</v>
       </c>
     </row>
     <row r="85">
@@ -1120,7 +1120,7 @@
         <v>43842.45833333334</v>
       </c>
       <c r="B85" t="n">
-        <v>0.04579374194145203</v>
+        <v>0.03548388183116913</v>
       </c>
     </row>
     <row r="86">
@@ -1128,7 +1128,7 @@
         <v>43842.5</v>
       </c>
       <c r="B86" t="n">
-        <v>0.05331335961818695</v>
+        <v>0.03743801638484001</v>
       </c>
     </row>
     <row r="87">
@@ -1136,7 +1136,7 @@
         <v>43842.54166666666</v>
       </c>
       <c r="B87" t="n">
-        <v>0.05276621878147125</v>
+        <v>0.03743801638484001</v>
       </c>
     </row>
     <row r="88">
@@ -1144,7 +1144,7 @@
         <v>43842.58333333334</v>
       </c>
       <c r="B88" t="n">
-        <v>0.04659110680222511</v>
+        <v>0.03264018148183823</v>
       </c>
     </row>
     <row r="89">
@@ -1152,7 +1152,7 @@
         <v>43842.625</v>
       </c>
       <c r="B89" t="n">
-        <v>0.04152054339647293</v>
+        <v>0.03034817613661289</v>
       </c>
     </row>
     <row r="90">
@@ -1160,7 +1160,7 @@
         <v>43842.66666666666</v>
       </c>
       <c r="B90" t="n">
-        <v>0.03426337242126465</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="91">
@@ -1168,7 +1168,7 @@
         <v>43842.70833333334</v>
       </c>
       <c r="B91" t="n">
-        <v>0.02449900284409523</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="92">
@@ -1176,7 +1176,7 @@
         <v>43842.75</v>
       </c>
       <c r="B92" t="n">
-        <v>0.02445698156952858</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="93">
@@ -1184,7 +1184,7 @@
         <v>43842.79166666666</v>
       </c>
       <c r="B93" t="n">
-        <v>0.02523075602948666</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
     <row r="94">
@@ -1192,7 +1192,7 @@
         <v>43842.83333333334</v>
       </c>
       <c r="B94" t="n">
-        <v>0.02478346787393093</v>
+        <v>0.02796140685677528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>